<commit_message>
error in New South Wales, Australia
was listed as its own parent causing an infinite recursion loop
</commit_message>
<xml_diff>
--- a/data/location_data.xlsx
+++ b/data/location_data.xlsx
@@ -7312,9 +7312,9 @@
   <dimension ref="A1:T1110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A1088" activePane="bottomLeft"/>
+      <pane ySplit="600" topLeftCell="A596" activePane="bottomLeft"/>
       <selection activeCell="B1" sqref="B1:C1048576"/>
-      <selection pane="bottomLeft" activeCell="A1115" sqref="A1115"/>
+      <selection pane="bottomLeft" activeCell="A617" sqref="A617"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31703,7 +31703,7 @@
         <v>7</v>
       </c>
       <c r="G617" s="3" t="s">
-        <v>59</v>
+        <v>787</v>
       </c>
       <c r="H617" s="3" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
March 2018 Monthly Update
</commit_message>
<xml_diff>
--- a/data/location_data.xlsx
+++ b/data/location_data.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox (Personal)\Webpages\TaxonomyMonographBuilder\fiddlercrab.info\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898ADB49-E6A9-44B5-93D5-4A23CF4EB1EC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2610" yWindow="720" windowWidth="22995" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">location_data!$A$1:$N$1384</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">location_data!$A$1:$N$1410</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15048" uniqueCount="2902">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15360" uniqueCount="2957">
   <si>
     <t>Latitude</t>
   </si>
@@ -8731,6 +8732,171 @@
   </si>
   <si>
     <t>Newport Bay, Newport Beach, Orange County, California, USA</t>
+  </si>
+  <si>
+    <t>Ishigaki, Okinawa, Ryukyu Islands, Japan</t>
+  </si>
+  <si>
+    <t>Ishigaki</t>
+  </si>
+  <si>
+    <t>Nagura River, Ishigaki, Okinawa, Ryukyu Islands, Japan</t>
+  </si>
+  <si>
+    <t>Nagura River</t>
+  </si>
+  <si>
+    <t>Nakakama River, Iriomote-jima, Okinawa, Ryukyu Islands, Japan</t>
+  </si>
+  <si>
+    <t>Nakakama River</t>
+  </si>
+  <si>
+    <t>Haemi, Iriomote-jima, Okinawa, Ryukyu Islands, Japan</t>
+  </si>
+  <si>
+    <t>Haemi</t>
+  </si>
+  <si>
+    <t>Ohara River</t>
+  </si>
+  <si>
+    <t>Ohara River, Haemi, Iriomote-jima, Okinawa, Ryukyu Islands, Japan</t>
+  </si>
+  <si>
+    <t>Nakamazaki, Iriomote-jima, Okinawa, Ryukyu Islands, Japan</t>
+  </si>
+  <si>
+    <t>Nakamazaki</t>
+  </si>
+  <si>
+    <t>Shirahama, Iriomote-jima, Okinawa, Ryukyu Islands, Japan</t>
+  </si>
+  <si>
+    <t>Shirahama</t>
+  </si>
+  <si>
+    <t>Ohara, Haemi, Iriomote-jima, Okinawa, Ryukyu Islands, Japan</t>
+  </si>
+  <si>
+    <t>Ohara</t>
+  </si>
+  <si>
+    <t>Saji River, Haemi, Iriomote-jima, Okinawa, Ryukyu Islands, Japan</t>
+  </si>
+  <si>
+    <t>Saji River</t>
+  </si>
+  <si>
+    <t>Location usure, but flows into Ohara</t>
+  </si>
+  <si>
+    <t>Dajia River</t>
+  </si>
+  <si>
+    <t>TaChia River</t>
+  </si>
+  <si>
+    <t>Taichung</t>
+  </si>
+  <si>
+    <t>Taichung, Taiwan</t>
+  </si>
+  <si>
+    <t>Dajia River, Taichung, Taiwan</t>
+  </si>
+  <si>
+    <t>Gaomei Wetlands, Taichung, Taiwan</t>
+  </si>
+  <si>
+    <t>Kaomei Wetlands</t>
+  </si>
+  <si>
+    <t>Gaomei Wetlands</t>
+  </si>
+  <si>
+    <t>Bahía Sucia</t>
+  </si>
+  <si>
+    <t>Bahía Sucia, Puerto Rico</t>
+  </si>
+  <si>
+    <t>Coroa Grande, Rio de Janeiro, Brazil</t>
+  </si>
+  <si>
+    <t>Coroa Grande</t>
+  </si>
+  <si>
+    <t>Yao Yai Island, Phang-nga, Thailand</t>
+  </si>
+  <si>
+    <t>Yao Yai Island</t>
+  </si>
+  <si>
+    <t>Krabi</t>
+  </si>
+  <si>
+    <t>Krabi, Thailand</t>
+  </si>
+  <si>
+    <t>Satun</t>
+  </si>
+  <si>
+    <t>Satun, Thailand</t>
+  </si>
+  <si>
+    <t>Chon Buri, Thailand</t>
+  </si>
+  <si>
+    <t>Chon Buri</t>
+  </si>
+  <si>
+    <t>Rayong, Thailand</t>
+  </si>
+  <si>
+    <t>Rayong</t>
+  </si>
+  <si>
+    <t>Samut Prakan, Thailand</t>
+  </si>
+  <si>
+    <t>Samut Prakan</t>
+  </si>
+  <si>
+    <t>Chumphon</t>
+  </si>
+  <si>
+    <t>Chumphon, Thailand</t>
+  </si>
+  <si>
+    <t>Pattani, Thailand</t>
+  </si>
+  <si>
+    <t>Pattani</t>
+  </si>
+  <si>
+    <t>Narathiwat</t>
+  </si>
+  <si>
+    <t>Narathiwat, Thailand</t>
+  </si>
+  <si>
+    <t>Chanthaburi, Thailand</t>
+  </si>
+  <si>
+    <t>Chanthaburi</t>
+  </si>
+  <si>
+    <t>Phetchaburi, Thailand</t>
+  </si>
+  <si>
+    <t>Phetchaburi</t>
+  </si>
+  <si>
+    <t>Nakhon Si Thammarat</t>
+  </si>
+  <si>
+    <t>Nakhon Si Thammarat, Thailand</t>
   </si>
 </sst>
 </file>
@@ -8815,7 +8981,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -8855,6 +9021,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -9196,14 +9368,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1384"/>
+  <dimension ref="A1:N1412"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="1" topLeftCell="A1199" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1212" sqref="A1212"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.140625" customWidth="1"/>
     <col min="2" max="2" width="13" style="22" customWidth="1"/>
@@ -70254,8 +70426,1155 @@
         <v>6</v>
       </c>
     </row>
+    <row r="1385" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1385" s="32" t="s">
+        <v>2902</v>
+      </c>
+      <c r="B1385" s="22">
+        <v>24.407776999999999</v>
+      </c>
+      <c r="C1385" s="22">
+        <v>124.192294</v>
+      </c>
+      <c r="D1385" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1385" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1385" s="33" t="s">
+        <v>2903</v>
+      </c>
+      <c r="G1385" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1385" s="32" t="s">
+        <v>1943</v>
+      </c>
+      <c r="I1385" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1385" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1385" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1385" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1385" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1385" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1386" s="32" t="s">
+        <v>2904</v>
+      </c>
+      <c r="B1386" s="22">
+        <v>24.400324000000001</v>
+      </c>
+      <c r="C1386" s="22">
+        <v>124.144706</v>
+      </c>
+      <c r="D1386" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1386" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1386" s="3" t="s">
+        <v>2905</v>
+      </c>
+      <c r="G1386" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1386" s="32" t="s">
+        <v>2902</v>
+      </c>
+      <c r="I1386" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1386" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1386" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1386" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1386" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1386" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1387" s="32" t="s">
+        <v>2906</v>
+      </c>
+      <c r="B1387" s="22">
+        <v>24.287683999999999</v>
+      </c>
+      <c r="C1387" s="22">
+        <v>123.871855</v>
+      </c>
+      <c r="D1387" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1387" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1387" s="33" t="s">
+        <v>2907</v>
+      </c>
+      <c r="G1387" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1387" s="30" t="s">
+        <v>1945</v>
+      </c>
+      <c r="I1387" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1387" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1387" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1387" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1387" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1387" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1388" s="32" t="s">
+        <v>2908</v>
+      </c>
+      <c r="B1388" s="22">
+        <v>24.271895000000001</v>
+      </c>
+      <c r="C1388" s="22">
+        <v>123.828957</v>
+      </c>
+      <c r="D1388" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1388" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1388" s="33" t="s">
+        <v>2909</v>
+      </c>
+      <c r="G1388" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1388" s="30" t="s">
+        <v>1945</v>
+      </c>
+      <c r="I1388" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1388" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1388" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1388" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1388" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1388" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1389" s="32" t="s">
+        <v>2911</v>
+      </c>
+      <c r="B1389" s="22">
+        <v>24.265557999999999</v>
+      </c>
+      <c r="C1389" s="22">
+        <v>123.88087299999999</v>
+      </c>
+      <c r="D1389" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1389" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1389" s="3" t="s">
+        <v>2910</v>
+      </c>
+      <c r="G1389" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1389" s="32" t="s">
+        <v>2908</v>
+      </c>
+      <c r="I1389" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1389" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1389" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1389" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1389" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1389" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1390" s="32" t="s">
+        <v>2912</v>
+      </c>
+      <c r="B1390" s="22">
+        <v>24.274135000000001</v>
+      </c>
+      <c r="C1390" s="22">
+        <v>123.902495</v>
+      </c>
+      <c r="D1390" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1390" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1390" s="33" t="s">
+        <v>2913</v>
+      </c>
+      <c r="G1390" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1390" s="30" t="s">
+        <v>1945</v>
+      </c>
+      <c r="I1390" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1390" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1390" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1390" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1390" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1390" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1391" s="32" t="s">
+        <v>2914</v>
+      </c>
+      <c r="B1391" s="22">
+        <v>24.359615000000002</v>
+      </c>
+      <c r="C1391" s="22">
+        <v>123.746559</v>
+      </c>
+      <c r="D1391" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1391" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1391" s="33" t="s">
+        <v>2915</v>
+      </c>
+      <c r="G1391" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1391" s="30" t="s">
+        <v>1945</v>
+      </c>
+      <c r="I1391" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1391" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1391" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1391" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1391" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1391" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1392" s="32" t="s">
+        <v>2916</v>
+      </c>
+      <c r="B1392" s="22">
+        <v>24.272199000000001</v>
+      </c>
+      <c r="C1392" s="22">
+        <v>123.88336</v>
+      </c>
+      <c r="D1392" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1392" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1392" s="33" t="s">
+        <v>2917</v>
+      </c>
+      <c r="G1392" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1392" s="32" t="s">
+        <v>2908</v>
+      </c>
+      <c r="I1392" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1392" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1392" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1392" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1392" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1392" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1393" s="32" t="s">
+        <v>2918</v>
+      </c>
+      <c r="B1393" s="22">
+        <v>24.272199000000001</v>
+      </c>
+      <c r="C1393" s="22">
+        <v>123.88336</v>
+      </c>
+      <c r="D1393" s="30" t="s">
+        <v>2920</v>
+      </c>
+      <c r="E1393" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1393" s="33" t="s">
+        <v>2919</v>
+      </c>
+      <c r="G1393" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1393" s="32" t="s">
+        <v>2916</v>
+      </c>
+      <c r="I1393" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1393" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1393" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1393" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1393" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1393" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1394" s="32" t="s">
+        <v>2925</v>
+      </c>
+      <c r="B1394" s="22">
+        <v>24.326426000000001</v>
+      </c>
+      <c r="C1394" s="22">
+        <v>120.565224</v>
+      </c>
+      <c r="D1394" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1394" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1394" s="3" t="s">
+        <v>2921</v>
+      </c>
+      <c r="G1394" s="3" t="s">
+        <v>2922</v>
+      </c>
+      <c r="H1394" s="32" t="s">
+        <v>2924</v>
+      </c>
+      <c r="I1394" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1394" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1394" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1394" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1394" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1394" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1395" s="32" t="s">
+        <v>2924</v>
+      </c>
+      <c r="B1395" s="22">
+        <v>24.326256000000001</v>
+      </c>
+      <c r="C1395" s="22">
+        <v>120.553476</v>
+      </c>
+      <c r="D1395" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1395" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1395" s="3" t="s">
+        <v>2923</v>
+      </c>
+      <c r="G1395" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1395" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="I1395" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1395" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1395" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1395" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1395" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1395" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1396" s="32" t="s">
+        <v>2926</v>
+      </c>
+      <c r="B1396" s="22">
+        <v>24.311903999999998</v>
+      </c>
+      <c r="C1396" s="22">
+        <v>120.54974300000001</v>
+      </c>
+      <c r="D1396" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1396" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1396" s="3" t="s">
+        <v>2928</v>
+      </c>
+      <c r="G1396" s="3" t="s">
+        <v>2927</v>
+      </c>
+      <c r="H1396" s="32" t="s">
+        <v>2924</v>
+      </c>
+      <c r="I1396" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1396" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1396" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1396" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1396" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1396" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1397" s="32" t="s">
+        <v>2930</v>
+      </c>
+      <c r="B1397" s="22">
+        <v>17.962233000000001</v>
+      </c>
+      <c r="C1397" s="22">
+        <v>-67.183820999999995</v>
+      </c>
+      <c r="D1397" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1397" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1397" s="32" t="s">
+        <v>2929</v>
+      </c>
+      <c r="G1397" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1397" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="I1397" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1397" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1397" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1397" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1397" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1397" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1398" s="30" t="s">
+        <v>2931</v>
+      </c>
+      <c r="B1398" s="22">
+        <v>-22.903687000000001</v>
+      </c>
+      <c r="C1398" s="22">
+        <v>-43.863487999999997</v>
+      </c>
+      <c r="D1398" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1398" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1398" s="3" t="s">
+        <v>2932</v>
+      </c>
+      <c r="G1398" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1398" s="30" t="s">
+        <v>348</v>
+      </c>
+      <c r="I1398" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1398" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1398" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1398" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1398" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1398" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1399" s="32" t="s">
+        <v>2933</v>
+      </c>
+      <c r="B1399" s="22">
+        <v>8.0057799999999997</v>
+      </c>
+      <c r="C1399" s="22">
+        <v>98.593380999999994</v>
+      </c>
+      <c r="D1399" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1399" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1399" s="16" t="s">
+        <v>2934</v>
+      </c>
+      <c r="G1399" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1399" s="32" t="s">
+        <v>1680</v>
+      </c>
+      <c r="I1399" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1399" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1399" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1399" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1399" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1399" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1400" s="32" t="s">
+        <v>2936</v>
+      </c>
+      <c r="B1400" s="22">
+        <v>8.0059629999999995</v>
+      </c>
+      <c r="C1400" s="22">
+        <v>98.948590999999993</v>
+      </c>
+      <c r="D1400" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1400" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1400" s="33" t="s">
+        <v>2935</v>
+      </c>
+      <c r="G1400" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1400" s="31" t="s">
+        <v>2439</v>
+      </c>
+      <c r="I1400" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1400" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1400" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1400" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1400" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1400" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1401" s="32" t="s">
+        <v>2938</v>
+      </c>
+      <c r="B1401" s="22">
+        <v>6.7213710000000004</v>
+      </c>
+      <c r="C1401" s="22">
+        <v>99.905745999999994</v>
+      </c>
+      <c r="D1401" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1401" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1401" s="33" t="s">
+        <v>2937</v>
+      </c>
+      <c r="G1401" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1401" s="31" t="s">
+        <v>2439</v>
+      </c>
+      <c r="I1401" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1401" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1401" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1401" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1401" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1401" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1402" s="30" t="s">
+        <v>2939</v>
+      </c>
+      <c r="B1402" s="22">
+        <v>13.163854000000001</v>
+      </c>
+      <c r="C1402" s="22">
+        <v>100.917452</v>
+      </c>
+      <c r="D1402" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1402" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1402" s="16" t="s">
+        <v>2940</v>
+      </c>
+      <c r="G1402" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1402" s="32" t="s">
+        <v>2440</v>
+      </c>
+      <c r="I1402" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1402" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1402" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1402" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1402" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1402" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1403" s="30" t="s">
+        <v>2941</v>
+      </c>
+      <c r="B1403" s="22">
+        <v>12.586899000000001</v>
+      </c>
+      <c r="C1403" s="22">
+        <v>101.420317</v>
+      </c>
+      <c r="D1403" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1403" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1403" s="16" t="s">
+        <v>2942</v>
+      </c>
+      <c r="G1403" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1403" s="32" t="s">
+        <v>2440</v>
+      </c>
+      <c r="I1403" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1403" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1403" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1403" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1403" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1403" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1404" s="30" t="s">
+        <v>2943</v>
+      </c>
+      <c r="B1404" s="22">
+        <v>13.556298999999999</v>
+      </c>
+      <c r="C1404" s="22">
+        <v>100.577839</v>
+      </c>
+      <c r="D1404" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1404" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1404" s="16" t="s">
+        <v>2944</v>
+      </c>
+      <c r="G1404" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1404" s="32" t="s">
+        <v>2440</v>
+      </c>
+      <c r="I1404" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1404" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1404" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1404" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1404" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1404" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1405" s="30" t="s">
+        <v>2946</v>
+      </c>
+      <c r="B1405" s="22">
+        <v>10.340699000000001</v>
+      </c>
+      <c r="C1405" s="22">
+        <v>99.149124</v>
+      </c>
+      <c r="D1405" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1405" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1405" s="16" t="s">
+        <v>2945</v>
+      </c>
+      <c r="G1405" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1405" s="32" t="s">
+        <v>2440</v>
+      </c>
+      <c r="I1405" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1405" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1405" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1405" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1405" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1405" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1406" s="30" t="s">
+        <v>2947</v>
+      </c>
+      <c r="B1406" s="22">
+        <v>6.8865879999999997</v>
+      </c>
+      <c r="C1406" s="22">
+        <v>101.307793</v>
+      </c>
+      <c r="D1406" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1406" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1406" s="16" t="s">
+        <v>2948</v>
+      </c>
+      <c r="G1406" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1406" s="32" t="s">
+        <v>2440</v>
+      </c>
+      <c r="I1406" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1406" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1406" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1406" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1406" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1406" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1407" s="30" t="s">
+        <v>2950</v>
+      </c>
+      <c r="B1407" s="22">
+        <v>6.3715380000000001</v>
+      </c>
+      <c r="C1407" s="22">
+        <v>101.917599</v>
+      </c>
+      <c r="D1407" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1407" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1407" s="3" t="s">
+        <v>2949</v>
+      </c>
+      <c r="G1407" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1407" s="32" t="s">
+        <v>2440</v>
+      </c>
+      <c r="I1407" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1407" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1407" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1407" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1407" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1407" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1408" s="30" t="s">
+        <v>2951</v>
+      </c>
+      <c r="B1408" s="22">
+        <v>12.527203</v>
+      </c>
+      <c r="C1408" s="22">
+        <v>102.0117</v>
+      </c>
+      <c r="D1408" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1408" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1408" s="33" t="s">
+        <v>2952</v>
+      </c>
+      <c r="G1408" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1408" s="32" t="s">
+        <v>2440</v>
+      </c>
+      <c r="I1408" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1408" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1408" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1408" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1408" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1408" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1409" s="30" t="s">
+        <v>2953</v>
+      </c>
+      <c r="B1409" s="22">
+        <v>12.949738999999999</v>
+      </c>
+      <c r="C1409" s="22">
+        <v>100.033761</v>
+      </c>
+      <c r="D1409" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1409" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1409" s="33" t="s">
+        <v>2954</v>
+      </c>
+      <c r="G1409" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1409" s="32" t="s">
+        <v>2440</v>
+      </c>
+      <c r="I1409" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1409" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1409" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1409" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1409" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1409" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1410" s="35" t="s">
+        <v>2956</v>
+      </c>
+      <c r="B1410" s="22">
+        <v>8.5812430000000006</v>
+      </c>
+      <c r="C1410" s="22">
+        <v>100.009213</v>
+      </c>
+      <c r="D1410" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1410" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1410" s="38" t="s">
+        <v>2955</v>
+      </c>
+      <c r="G1410" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1410" s="37" t="s">
+        <v>2440</v>
+      </c>
+      <c r="I1410" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1410" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1410" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1410" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1410" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1410" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1412" s="36"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:N1384" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:N1410" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState ref="A360:N1155">
       <sortCondition ref="C1:C1235"/>
     </sortState>

</xml_diff>

<commit_message>
Nov 2019 update: includes newly designed range maps
</commit_message>
<xml_diff>
--- a/data/location_data.xlsx
+++ b/data/location_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Webpages\TaxonomyMonographBuilder\fiddlercrab.info\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E15FFD2-5490-42A0-9376-87CDF55D9657}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0390BBD-8A9B-40BC-AB56-4A2E33AFDC3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31056" yWindow="180" windowWidth="26412" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="396" yWindow="624" windowWidth="16548" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="location_data" sheetId="1" r:id="rId1"/>
@@ -12389,8 +12389,8 @@
   <dimension ref="A1:O23577"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1889" sqref="A1889"/>
+      <pane ySplit="1" topLeftCell="A1717" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1736" sqref="C1736"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -88924,8 +88924,8 @@
         <v>-5.4975000000000005</v>
       </c>
       <c r="C1736" s="10">
-        <f>125+45/60+21/3600</f>
-        <v>125.75583333333333</v>
+        <f>123.759761</f>
+        <v>123.759761</v>
       </c>
       <c r="D1736" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Mar 2020 update. Public release of size data
</commit_message>
<xml_diff>
--- a/data/location_data.xlsx
+++ b/data/location_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Webpages\TaxonomyMonographBuilder\fiddlercrab.info\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBB6E48-6514-403B-942B-65ABDA0FC53D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FAABA3-8AF6-489F-B3AD-EE18CEA27923}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12432" yWindow="96" windowWidth="18240" windowHeight="16572" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9984" yWindow="96" windowWidth="20244" windowHeight="14388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="location_data" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">location_data!$A$1:$N$1928</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">location_data!$A$1:$N$1939</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21448" uniqueCount="4049">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21580" uniqueCount="4071">
   <si>
     <t>Latitude</t>
   </si>
@@ -12183,6 +12183,72 @@
   </si>
   <si>
     <t>Knysna Lagoon, Western Cape, South Africa</t>
+  </si>
+  <si>
+    <t>Yinhai, Beihai, Guangxi, China</t>
+  </si>
+  <si>
+    <t>Yinhai</t>
+  </si>
+  <si>
+    <t>Alagoas, Brazil</t>
+  </si>
+  <si>
+    <t>Alagoas</t>
+  </si>
+  <si>
+    <t>Mundaú Lagoon, Alagoas, Brazil</t>
+  </si>
+  <si>
+    <t>Mundaú Lagoon</t>
+  </si>
+  <si>
+    <t>Pulicat Lake</t>
+  </si>
+  <si>
+    <t>Pulicat Lake, India</t>
+  </si>
+  <si>
+    <t>Rushikulya Estuary, Odisha, India</t>
+  </si>
+  <si>
+    <t>Rushikulya Estuary</t>
+  </si>
+  <si>
+    <t>Chinnapalam</t>
+  </si>
+  <si>
+    <t>Chinnapalam, Ramanathapuram District, Tamil Nadu, India</t>
+  </si>
+  <si>
+    <t>Kamboi, Gujarat, India</t>
+  </si>
+  <si>
+    <t>Kamboi</t>
+  </si>
+  <si>
+    <t>Nada, Gujarat, India</t>
+  </si>
+  <si>
+    <t>Nada</t>
+  </si>
+  <si>
+    <t>Gandhar, Gujarat, India</t>
+  </si>
+  <si>
+    <t>Gandhar</t>
+  </si>
+  <si>
+    <t>Tar Landing Bay, Beaufort, Carteret County, North Carolina, USA</t>
+  </si>
+  <si>
+    <t>Tar Landing Bay</t>
+  </si>
+  <si>
+    <t>Canary Creek Marsh, Lewes, Sussex County, Delaware, USA</t>
+  </si>
+  <si>
+    <t>Canary Creek Marsh</t>
   </si>
 </sst>
 </file>
@@ -12640,8 +12706,8 @@
   <dimension ref="A1:O23576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A138" sqref="A138"/>
+      <pane ySplit="1" topLeftCell="A1906" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1939" sqref="A1939"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -97676,19 +97742,495 @@
       </c>
     </row>
     <row r="1929" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1929" s="4"/>
+      <c r="A1929" t="s">
+        <v>4049</v>
+      </c>
+      <c r="B1929" s="10">
+        <f>21+24/60+31/3600</f>
+        <v>21.40861111111111</v>
+      </c>
+      <c r="C1929" s="10">
+        <f>109+12/60+2/3600</f>
+        <v>109.20055555555555</v>
+      </c>
+      <c r="D1929" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1929" s="3" t="s">
+        <v>1567</v>
+      </c>
+      <c r="F1929" s="3" t="s">
+        <v>4050</v>
+      </c>
+      <c r="G1929" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1929" t="s">
+        <v>3208</v>
+      </c>
+      <c r="I1929" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1929" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1929" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1929" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1929" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1929" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="1930" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1930" s="4"/>
+      <c r="A1930" t="s">
+        <v>4051</v>
+      </c>
+      <c r="B1930" s="10">
+        <v>-9.5599349999999994</v>
+      </c>
+      <c r="C1930" s="10">
+        <v>-35.720379000000001</v>
+      </c>
+      <c r="D1930" t="s">
+        <v>2207</v>
+      </c>
+      <c r="E1930" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1930" s="3" t="s">
+        <v>4052</v>
+      </c>
+      <c r="G1930" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1930" t="s">
+        <v>327</v>
+      </c>
+      <c r="I1930" t="s">
+        <v>329</v>
+      </c>
+      <c r="J1930" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1930" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1930" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1930" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1930" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1931" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1931" t="s">
+        <v>4053</v>
+      </c>
+      <c r="B1931" s="10">
+        <v>-9.6263869999999994</v>
+      </c>
+      <c r="C1931" s="10">
+        <v>-35.778005</v>
+      </c>
+      <c r="D1931" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1931" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1931" s="3" t="s">
+        <v>4054</v>
+      </c>
+      <c r="G1931" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1931" t="s">
+        <v>4051</v>
+      </c>
+      <c r="I1931" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1931" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1931" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1931" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1931" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1931" s="13" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="1932" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1932" s="4"/>
+      <c r="A1932" s="4" t="s">
+        <v>4056</v>
+      </c>
+      <c r="B1932" s="10">
+        <v>13.599276</v>
+      </c>
+      <c r="C1932" s="10">
+        <v>80.186243000000005</v>
+      </c>
+      <c r="D1932" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1932" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1932" s="3" t="s">
+        <v>4055</v>
+      </c>
+      <c r="G1932" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1932" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="I1932" s="3" t="s">
+        <v>3643</v>
+      </c>
+      <c r="J1932" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1932" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1932" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1932" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1932" s="13" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="1933" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1933" s="4"/>
+      <c r="A1933" t="s">
+        <v>4057</v>
+      </c>
+      <c r="B1933" s="10">
+        <v>19.380182000000001</v>
+      </c>
+      <c r="C1933" s="10">
+        <v>85.040762999999998</v>
+      </c>
+      <c r="D1933" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1933" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1933" s="3" t="s">
+        <v>4058</v>
+      </c>
+      <c r="G1933" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1933" t="s">
+        <v>2347</v>
+      </c>
+      <c r="I1933" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1933" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1933" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1933" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1933" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1933" s="13" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="1934" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1934" s="4"/>
+      <c r="A1934" t="s">
+        <v>4060</v>
+      </c>
+      <c r="B1934" s="10">
+        <f>9+16/60</f>
+        <v>9.2666666666666675</v>
+      </c>
+      <c r="C1934" s="10">
+        <f>79+13/60</f>
+        <v>79.216666666666669</v>
+      </c>
+      <c r="D1934" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1934" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1934" s="4" t="s">
+        <v>4059</v>
+      </c>
+      <c r="G1934" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1934" t="s">
+        <v>2333</v>
+      </c>
+      <c r="I1934" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1934" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1934" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1934" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1934" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1934" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1935" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1935" t="s">
+        <v>4061</v>
+      </c>
+      <c r="B1935" s="10">
+        <v>22.216901</v>
+      </c>
+      <c r="C1935" s="10">
+        <v>72.621713999999997</v>
+      </c>
+      <c r="D1935" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1935" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1935" s="3" t="s">
+        <v>4062</v>
+      </c>
+      <c r="G1935" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1935" t="s">
+        <v>2368</v>
+      </c>
+      <c r="I1935" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1935" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1935" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1935" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1935" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1935" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1936" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1936" t="s">
+        <v>4063</v>
+      </c>
+      <c r="B1936" s="10">
+        <v>21.922920999999999</v>
+      </c>
+      <c r="C1936" s="10">
+        <v>72.512658999999999</v>
+      </c>
+      <c r="D1936" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1936" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1936" s="3" t="s">
+        <v>4064</v>
+      </c>
+      <c r="G1936" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1936" t="s">
+        <v>2368</v>
+      </c>
+      <c r="I1936" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1936" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1936" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1936" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1936" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1936" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1937" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1937" t="s">
+        <v>4065</v>
+      </c>
+      <c r="B1937" s="10">
+        <v>21.901105999999999</v>
+      </c>
+      <c r="C1937" s="10">
+        <v>72.625575999999995</v>
+      </c>
+      <c r="D1937" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1937" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1937" s="3" t="s">
+        <v>4066</v>
+      </c>
+      <c r="G1937" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1937" t="s">
+        <v>2368</v>
+      </c>
+      <c r="I1937" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1937" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1937" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1937" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1937" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1937" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1938" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1938" t="s">
+        <v>4067</v>
+      </c>
+      <c r="B1938" s="10">
+        <v>34.701917000000002</v>
+      </c>
+      <c r="C1938" s="10">
+        <v>-76.704702999999995</v>
+      </c>
+      <c r="D1938" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1938" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1938" s="3" t="s">
+        <v>4068</v>
+      </c>
+      <c r="G1938" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1938" t="s">
+        <v>2619</v>
+      </c>
+      <c r="I1938" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1938" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1938" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1938" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1938" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1938" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1939" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1939" t="s">
+        <v>4069</v>
+      </c>
+      <c r="B1939" s="10">
+        <v>38.788542999999997</v>
+      </c>
+      <c r="C1939" s="10">
+        <v>-75.165891999999999</v>
+      </c>
+      <c r="D1939" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1939" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1939" s="3" t="s">
+        <v>4070</v>
+      </c>
+      <c r="G1939" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1939" t="s">
+        <v>633</v>
+      </c>
+      <c r="I1939" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1939" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1939" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1939" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1939" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1939" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1941" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1941" s="4"/>
     </row>
     <row r="23576" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23576" t="s">
@@ -97696,7 +98238,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N1928" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:N1939" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N1869">
       <sortCondition sortBy="cellColor" ref="A1:A1869" dxfId="0"/>
     </sortState>

</xml_diff>

<commit_message>
July 2020 update - includes reworking of name updates for non-species names (genera, etc)
</commit_message>
<xml_diff>
--- a/data/location_data.xlsx
+++ b/data/location_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\Webpages\TaxonomyMonographBuilder\fiddlercrab.info\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A53D4F2-B403-4B63-B4EB-3679E3873906}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB00854-67A6-4311-98C2-1562DB82231D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="90" windowWidth="19455" windowHeight="20820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="405" windowWidth="21885" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="location_data" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">location_data!$A$1:$J$2068</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">location_data!$A$1:$J$2099</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16553" uniqueCount="4330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16801" uniqueCount="4392">
   <si>
     <t>Latitude</t>
   </si>
@@ -13026,6 +13026,192 @@
   </si>
   <si>
     <t>Sabine National Wildlife Refuge, Cameron Parish, Louisiana, USA</t>
+  </si>
+  <si>
+    <t>Port Henderson, Jamaica</t>
+  </si>
+  <si>
+    <t>Port Henderson</t>
+  </si>
+  <si>
+    <t>Mantanzas, Cuba</t>
+  </si>
+  <si>
+    <t>Mantanzas</t>
+  </si>
+  <si>
+    <t>Nassau County, Florida, USA</t>
+  </si>
+  <si>
+    <t>Nassau County</t>
+  </si>
+  <si>
+    <t>Fernandina Beach, Nassau County, Florida, USA</t>
+  </si>
+  <si>
+    <t>Fernandina Beach</t>
+  </si>
+  <si>
+    <t>Volusia County, Florida, USA</t>
+  </si>
+  <si>
+    <t>Volusia County</t>
+  </si>
+  <si>
+    <t>Callalisa Park</t>
+  </si>
+  <si>
+    <t>Callalisa Park, Volusia County, Florida, USA</t>
+  </si>
+  <si>
+    <t>Hollywood</t>
+  </si>
+  <si>
+    <t>Broward County, Florida, USA</t>
+  </si>
+  <si>
+    <t>Broward County</t>
+  </si>
+  <si>
+    <t>Hollywood, Broward County, Florida, USA</t>
+  </si>
+  <si>
+    <t>Campeche, Mexico</t>
+  </si>
+  <si>
+    <t>Campeche</t>
+  </si>
+  <si>
+    <t>Campeche (State)</t>
+  </si>
+  <si>
+    <t>Campeche, Campeche, Mexico</t>
+  </si>
+  <si>
+    <t>Champoton, Campeche, Mexico</t>
+  </si>
+  <si>
+    <t>Champoton</t>
+  </si>
+  <si>
+    <t>Amapá, Brazil</t>
+  </si>
+  <si>
+    <t>Amapá</t>
+  </si>
+  <si>
+    <t>Rio Amapá, Amapá, Brazil</t>
+  </si>
+  <si>
+    <t>Rio Amapá</t>
+  </si>
+  <si>
+    <t>Salinópolis, Pará, Brazil</t>
+  </si>
+  <si>
+    <t>Salinópolis</t>
+  </si>
+  <si>
+    <t>Icatu, Maranhão, Brazil</t>
+  </si>
+  <si>
+    <t>Icatu</t>
+  </si>
+  <si>
+    <t>Ilha de Itamaracá</t>
+  </si>
+  <si>
+    <t>Ilha de Itamaracá, Pernambuco, Brazil</t>
+  </si>
+  <si>
+    <t>Sirinhaém</t>
+  </si>
+  <si>
+    <t>Sirinhaém, Pernambuco, Brazil</t>
+  </si>
+  <si>
+    <t>Rio Camaragibe</t>
+  </si>
+  <si>
+    <t>Rio Camaragibe, Alagoas, Brazil</t>
+  </si>
+  <si>
+    <t>Porto do Sauipe, Bahia, Brazil</t>
+  </si>
+  <si>
+    <t>Porto do Sauipe</t>
+  </si>
+  <si>
+    <t>Guarapari, Espírito Santo, Brazil</t>
+  </si>
+  <si>
+    <t>Guarapari</t>
+  </si>
+  <si>
+    <t>Marataízes</t>
+  </si>
+  <si>
+    <t>Marataízes, Espírito Santo, Brazil</t>
+  </si>
+  <si>
+    <t>Bertioga, São Paulo, Brazil</t>
+  </si>
+  <si>
+    <t>Bertioga</t>
+  </si>
+  <si>
+    <t>Cananéia</t>
+  </si>
+  <si>
+    <t>Cananéia, São Paulo, Brazil</t>
+  </si>
+  <si>
+    <t>Guaratuba, Paraná, Brazil</t>
+  </si>
+  <si>
+    <t>Guaratuba</t>
+  </si>
+  <si>
+    <t>Santa Catarina, Brazil</t>
+  </si>
+  <si>
+    <t>Santa Catarina</t>
+  </si>
+  <si>
+    <t>Florianópolis</t>
+  </si>
+  <si>
+    <t>Florianópolis, Santa Catarina, Brazil</t>
+  </si>
+  <si>
+    <t>Okukubi River, Okinawa, Ryukyu Islands, Japan</t>
+  </si>
+  <si>
+    <t>Okukubi River</t>
+  </si>
+  <si>
+    <t>Pwani Region, Tanzania</t>
+  </si>
+  <si>
+    <t>Pwani Region</t>
+  </si>
+  <si>
+    <t>Rufiji River, Pwani Region, Tanzania</t>
+  </si>
+  <si>
+    <t>Rufiji River</t>
+  </si>
+  <si>
+    <t>Ras Dege Estuary, Dar es Salaam, Tanzania</t>
+  </si>
+  <si>
+    <t>Ras Dege Estuary</t>
+  </si>
+  <si>
+    <t>Bocaripo Lagoon, Sucre, Venezuela</t>
+  </si>
+  <si>
+    <t>Bocaripo Lagoon</t>
   </si>
 </sst>
 </file>
@@ -13478,11 +13664,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2068"/>
+  <dimension ref="A1:K2101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A1:J2068"/>
+      <pane ySplit="1" topLeftCell="A2049" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2099" sqref="A2099"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -79923,8 +80109,1005 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2069" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2069" t="s">
+        <v>4330</v>
+      </c>
+      <c r="B2069" s="10">
+        <v>17.949214999999999</v>
+      </c>
+      <c r="C2069" s="10">
+        <v>-76.874409</v>
+      </c>
+      <c r="D2069" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2069" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2069" s="3" t="s">
+        <v>4331</v>
+      </c>
+      <c r="G2069" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2069" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="I2069" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2069" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2070" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2070" t="s">
+        <v>4332</v>
+      </c>
+      <c r="B2070" s="10">
+        <v>23.038824999999999</v>
+      </c>
+      <c r="C2070" s="10">
+        <v>-81.544044999999997</v>
+      </c>
+      <c r="D2070" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2070" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2070" s="3" t="s">
+        <v>4333</v>
+      </c>
+      <c r="G2070" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2070" t="s">
+        <v>306</v>
+      </c>
+      <c r="I2070" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2070" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2071" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2071" t="s">
+        <v>4334</v>
+      </c>
+      <c r="B2071" s="10">
+        <v>30.610468000000001</v>
+      </c>
+      <c r="C2071" s="10">
+        <v>-81.441631999999998</v>
+      </c>
+      <c r="D2071" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2071" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2071" s="3" t="s">
+        <v>4335</v>
+      </c>
+      <c r="G2071" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2071" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="I2071" t="s">
+        <v>310</v>
+      </c>
+      <c r="J2071" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2072" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2072" t="s">
+        <v>4336</v>
+      </c>
+      <c r="B2072" s="10">
+        <v>30.647597000000001</v>
+      </c>
+      <c r="C2072" s="10">
+        <v>-81.434471000000002</v>
+      </c>
+      <c r="D2072" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2072" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2072" s="3" t="s">
+        <v>4337</v>
+      </c>
+      <c r="G2072" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2072" t="s">
+        <v>4334</v>
+      </c>
+      <c r="I2072" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2072" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2073" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2073" t="s">
+        <v>4338</v>
+      </c>
+      <c r="B2073" s="10">
+        <v>29.077494000000002</v>
+      </c>
+      <c r="C2073" s="10">
+        <v>-80.923625999999999</v>
+      </c>
+      <c r="D2073" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2073" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2073" s="3" t="s">
+        <v>4339</v>
+      </c>
+      <c r="G2073" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2073" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="I2073" t="s">
+        <v>310</v>
+      </c>
+      <c r="J2073" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2074" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2074" t="s">
+        <v>4341</v>
+      </c>
+      <c r="B2074" s="10">
+        <v>29.029509999999998</v>
+      </c>
+      <c r="C2074" s="10">
+        <v>-80.904216000000005</v>
+      </c>
+      <c r="D2074" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2074" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2074" s="3" t="s">
+        <v>4340</v>
+      </c>
+      <c r="G2074" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2074" t="s">
+        <v>4338</v>
+      </c>
+      <c r="I2074" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2074" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2075" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2075" t="s">
+        <v>4345</v>
+      </c>
+      <c r="B2075" s="10">
+        <v>26.022015</v>
+      </c>
+      <c r="C2075" s="10">
+        <v>-80.114267999999996</v>
+      </c>
+      <c r="D2075" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2075" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2075" s="3" t="s">
+        <v>4342</v>
+      </c>
+      <c r="G2075" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2075" t="s">
+        <v>4343</v>
+      </c>
+      <c r="I2075" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2075" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2076" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2076" t="s">
+        <v>4343</v>
+      </c>
+      <c r="B2076" s="10">
+        <v>26.157446</v>
+      </c>
+      <c r="C2076" s="10">
+        <v>-80.997110000000006</v>
+      </c>
+      <c r="D2076" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2076" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2076" s="3" t="s">
+        <v>4344</v>
+      </c>
+      <c r="G2076" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2076" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="I2076" t="s">
+        <v>310</v>
+      </c>
+      <c r="J2076" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2077" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2077" t="s">
+        <v>4346</v>
+      </c>
+      <c r="B2077" s="10">
+        <v>19.209285000000001</v>
+      </c>
+      <c r="C2077" s="10">
+        <v>-90.877838999999994</v>
+      </c>
+      <c r="D2077" t="s">
+        <v>2198</v>
+      </c>
+      <c r="E2077" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2077" s="3" t="s">
+        <v>4348</v>
+      </c>
+      <c r="G2077" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2077" t="s">
+        <v>2155</v>
+      </c>
+      <c r="I2077" t="s">
+        <v>447</v>
+      </c>
+      <c r="J2077" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2078" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2078" t="s">
+        <v>4349</v>
+      </c>
+      <c r="B2078" s="10">
+        <v>19.846705</v>
+      </c>
+      <c r="C2078" s="10">
+        <v>-90.541385000000005</v>
+      </c>
+      <c r="D2078" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2078" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2078" s="3" t="s">
+        <v>4347</v>
+      </c>
+      <c r="G2078" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2078" t="s">
+        <v>4346</v>
+      </c>
+      <c r="I2078" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2078" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2079" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2079" t="s">
+        <v>4350</v>
+      </c>
+      <c r="B2079" s="10">
+        <v>19.346592999999999</v>
+      </c>
+      <c r="C2079" s="10">
+        <v>-90.731435000000005</v>
+      </c>
+      <c r="D2079" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2079" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2079" s="3" t="s">
+        <v>4351</v>
+      </c>
+      <c r="G2079" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2079" t="s">
+        <v>4346</v>
+      </c>
+      <c r="I2079" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2079" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2080" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2080" t="s">
+        <v>4352</v>
+      </c>
+      <c r="B2080" s="10">
+        <v>2.5051860000000001</v>
+      </c>
+      <c r="C2080" s="10">
+        <v>-50.819522999999997</v>
+      </c>
+      <c r="D2080" t="s">
+        <v>2198</v>
+      </c>
+      <c r="E2080" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2080" s="3" t="s">
+        <v>4353</v>
+      </c>
+      <c r="G2080" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2080" t="s">
+        <v>327</v>
+      </c>
+      <c r="I2080" t="s">
+        <v>331</v>
+      </c>
+      <c r="J2080" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2081" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2081" t="s">
+        <v>4354</v>
+      </c>
+      <c r="B2081" s="10">
+        <v>2.137432</v>
+      </c>
+      <c r="C2081" s="10">
+        <v>-50.704255000000003</v>
+      </c>
+      <c r="D2081" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2081" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2081" s="3" t="s">
+        <v>4355</v>
+      </c>
+      <c r="G2081" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2081" t="s">
+        <v>4352</v>
+      </c>
+      <c r="I2081" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2081" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2082" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2082" t="s">
+        <v>4356</v>
+      </c>
+      <c r="B2082" s="10">
+        <v>-0.61447799999999997</v>
+      </c>
+      <c r="C2082" s="10">
+        <v>-47.349525999999997</v>
+      </c>
+      <c r="D2082" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2082" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2082" t="s">
+        <v>4357</v>
+      </c>
+      <c r="G2082" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2082" t="s">
+        <v>332</v>
+      </c>
+      <c r="I2082" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2082" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2083" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2083" t="s">
+        <v>4358</v>
+      </c>
+      <c r="B2083" s="10">
+        <v>-2.7756289999999999</v>
+      </c>
+      <c r="C2083" s="10">
+        <v>-44.067132999999998</v>
+      </c>
+      <c r="D2083" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2083" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2083" s="3" t="s">
+        <v>4359</v>
+      </c>
+      <c r="G2083" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2083" t="s">
+        <v>352</v>
+      </c>
+      <c r="I2083" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2083" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2084" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2084" t="s">
+        <v>4361</v>
+      </c>
+      <c r="B2084" s="10">
+        <v>-7.7638550000000004</v>
+      </c>
+      <c r="C2084" s="10">
+        <v>-34.828212999999998</v>
+      </c>
+      <c r="D2084" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2084" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2084" s="3" t="s">
+        <v>4360</v>
+      </c>
+      <c r="G2084" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2084" t="s">
+        <v>333</v>
+      </c>
+      <c r="I2084" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2084" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2085" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2085" t="s">
+        <v>4363</v>
+      </c>
+      <c r="B2085" s="10">
+        <v>-8.6202199999999998</v>
+      </c>
+      <c r="C2085" s="10">
+        <v>-35.055526999999998</v>
+      </c>
+      <c r="D2085" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2085" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2085" s="3" t="s">
+        <v>4362</v>
+      </c>
+      <c r="G2085" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2085" t="s">
+        <v>333</v>
+      </c>
+      <c r="I2085" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2085" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2086" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2086" t="s">
+        <v>4365</v>
+      </c>
+      <c r="B2086" s="10">
+        <v>-9.3131310000000003</v>
+      </c>
+      <c r="C2086" s="10">
+        <v>-35.429212999999997</v>
+      </c>
+      <c r="D2086" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2086" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2086" s="3" t="s">
+        <v>4364</v>
+      </c>
+      <c r="G2086" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2086" t="s">
+        <v>4036</v>
+      </c>
+      <c r="I2086" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2086" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2087" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2087" t="s">
+        <v>4366</v>
+      </c>
+      <c r="B2087" s="10">
+        <v>-12.390040000000001</v>
+      </c>
+      <c r="C2087" s="10">
+        <v>-37.880358999999999</v>
+      </c>
+      <c r="D2087" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2087" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2087" s="3" t="s">
+        <v>4367</v>
+      </c>
+      <c r="G2087" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2087" t="s">
+        <v>326</v>
+      </c>
+      <c r="I2087" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2087" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2088" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2088" t="s">
+        <v>4368</v>
+      </c>
+      <c r="B2088" s="10">
+        <v>-20.67597</v>
+      </c>
+      <c r="C2088" s="10">
+        <v>-40.50159</v>
+      </c>
+      <c r="D2088" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2088" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2088" s="3" t="s">
+        <v>4369</v>
+      </c>
+      <c r="G2088" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2088" t="s">
+        <v>339</v>
+      </c>
+      <c r="I2088" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2088" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2089" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2089" t="s">
+        <v>4371</v>
+      </c>
+      <c r="B2089" s="10">
+        <v>-21.046327999999999</v>
+      </c>
+      <c r="C2089" s="10">
+        <v>-40.828198</v>
+      </c>
+      <c r="D2089" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2089" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2089" s="3" t="s">
+        <v>4370</v>
+      </c>
+      <c r="G2089" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2089" t="s">
+        <v>339</v>
+      </c>
+      <c r="I2089" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2089" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2090" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2090" t="s">
+        <v>4372</v>
+      </c>
+      <c r="B2090" s="10">
+        <v>-23.83625</v>
+      </c>
+      <c r="C2090" s="10">
+        <v>-45.119155999999997</v>
+      </c>
+      <c r="D2090" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2090" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2090" s="3" t="s">
+        <v>4373</v>
+      </c>
+      <c r="G2090" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2090" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="I2090" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2090" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2091" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2091" t="s">
+        <v>4375</v>
+      </c>
+      <c r="B2091" s="10">
+        <v>-25.013652</v>
+      </c>
+      <c r="C2091" s="10">
+        <v>-47.926667999999999</v>
+      </c>
+      <c r="D2091" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2091" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2091" s="3" t="s">
+        <v>4374</v>
+      </c>
+      <c r="G2091" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2091" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="I2091" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2091" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2092" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2092" t="s">
+        <v>4376</v>
+      </c>
+      <c r="B2092" s="10">
+        <v>-25.881722</v>
+      </c>
+      <c r="C2092" s="10">
+        <v>-48.567810000000001</v>
+      </c>
+      <c r="D2092" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2092" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2092" s="3" t="s">
+        <v>4377</v>
+      </c>
+      <c r="G2092" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2092" t="s">
+        <v>336</v>
+      </c>
+      <c r="I2092" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2092" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2093" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2093" t="s">
+        <v>4378</v>
+      </c>
+      <c r="B2093" s="10">
+        <v>-27.545074</v>
+      </c>
+      <c r="C2093" s="10">
+        <v>-48.657190999999997</v>
+      </c>
+      <c r="D2093" t="s">
+        <v>2198</v>
+      </c>
+      <c r="E2093" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2093" s="3" t="s">
+        <v>4379</v>
+      </c>
+      <c r="G2093" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2093" t="s">
+        <v>327</v>
+      </c>
+      <c r="I2093" t="s">
+        <v>2118</v>
+      </c>
+      <c r="J2093" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2094" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2094" t="s">
+        <v>4381</v>
+      </c>
+      <c r="B2094" s="10">
+        <v>-27.600128000000002</v>
+      </c>
+      <c r="C2094" s="10">
+        <v>-48.482644000000001</v>
+      </c>
+      <c r="D2094" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2094" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2094" s="3" t="s">
+        <v>4380</v>
+      </c>
+      <c r="G2094" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2094" t="s">
+        <v>4378</v>
+      </c>
+      <c r="I2094" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2094" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2095" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2095" t="s">
+        <v>4382</v>
+      </c>
+      <c r="B2095" s="10">
+        <v>26.454808</v>
+      </c>
+      <c r="C2095" s="10">
+        <v>127.944007</v>
+      </c>
+      <c r="D2095" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2095" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2095" s="3" t="s">
+        <v>4383</v>
+      </c>
+      <c r="G2095" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2095" t="s">
+        <v>1902</v>
+      </c>
+      <c r="I2095" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2095" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2096" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2096" t="s">
+        <v>4384</v>
+      </c>
+      <c r="B2096" s="10">
+        <v>-7.3096059999999996</v>
+      </c>
+      <c r="C2096" s="10">
+        <v>39.369404000000003</v>
+      </c>
+      <c r="D2096" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2096" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2096" s="3" t="s">
+        <v>4385</v>
+      </c>
+      <c r="G2096" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2096" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2096" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2096" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2097" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2097" t="s">
+        <v>4386</v>
+      </c>
+      <c r="B2097" s="10">
+        <v>-7.8045229999999997</v>
+      </c>
+      <c r="C2097" s="10">
+        <v>39.326158999999997</v>
+      </c>
+      <c r="D2097" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2097" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2097" s="3" t="s">
+        <v>4387</v>
+      </c>
+      <c r="G2097" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2097" t="s">
+        <v>4384</v>
+      </c>
+      <c r="I2097" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2097" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2098" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2098" t="s">
+        <v>4388</v>
+      </c>
+      <c r="B2098" s="10">
+        <v>-6.8103899999999999</v>
+      </c>
+      <c r="C2098" s="10">
+        <v>39.452007999999999</v>
+      </c>
+      <c r="D2098" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2098" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2098" s="3" t="s">
+        <v>4389</v>
+      </c>
+      <c r="G2098" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2098" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2098" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2098" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2099" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2099" t="s">
+        <v>4390</v>
+      </c>
+      <c r="B2099" s="10">
+        <f>10+35/60</f>
+        <v>10.583333333333334</v>
+      </c>
+      <c r="C2099" s="10">
+        <f>-(65+2.5/60)</f>
+        <v>-65.041666666666671</v>
+      </c>
+      <c r="D2099" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2099" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2099" s="3" t="s">
+        <v>4391</v>
+      </c>
+      <c r="G2099" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2099" s="4" t="s">
+        <v>1709</v>
+      </c>
+      <c r="I2099" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2099" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2101" s="4"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J2068" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:J2099" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J1869">
       <sortCondition sortBy="cellColor" ref="A1:A1869" dxfId="0"/>
     </sortState>

</xml_diff>